<commit_message>
removed messagebox in sub1 added logic for days selection
</commit_message>
<xml_diff>
--- a/stutechclass.xlsx
+++ b/stutechclass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JINALI\Documents\UiPath\Teacher_Student_Classbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C8B0D9-FC0D-40CD-960F-D6320D321F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1AF2B7-E5BF-4E7E-8530-A3017BB2D291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -321,6 +321,36 @@
   </si>
   <si>
     <t xml:space="preserve">Thu  </t>
+  </si>
+  <si>
+    <t>Abc1 Xyz1</t>
+  </si>
+  <si>
+    <t>Abc2 Xyz2</t>
+  </si>
+  <si>
+    <t>Abc3 Xyz3</t>
+  </si>
+  <si>
+    <t>Abc4 Xyz4</t>
+  </si>
+  <si>
+    <t>Abc5 Xyz5</t>
+  </si>
+  <si>
+    <t>Abc6 Xyz6</t>
+  </si>
+  <si>
+    <t>Abc7 Xyz7</t>
+  </si>
+  <si>
+    <t>Abc8 Xyz8</t>
+  </si>
+  <si>
+    <t>Abc9 Xyz9</t>
+  </si>
+  <si>
+    <t>Abc10 Xyz10</t>
   </si>
 </sst>
 </file>
@@ -668,7 +698,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="263" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +917,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="211" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +960,7 @@
         <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -947,7 +977,7 @@
         <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -964,7 +994,7 @@
         <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -981,7 +1011,7 @@
         <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,7 +1028,7 @@
         <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1015,7 +1045,7 @@
         <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1032,7 +1062,7 @@
         <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1049,7 +1079,7 @@
         <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1066,7 +1096,7 @@
         <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1083,7 +1113,7 @@
         <v>93</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1127,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A12" sqref="A12:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>